<commit_message>
FIX: add school username
</commit_message>
<xml_diff>
--- a/src/assets/SchoolTrackBulkUpload.xlsx
+++ b/src/assets/SchoolTrackBulkUpload.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23930"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1158A278-880D-4692-A27F-0BD1C60CD226}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{16EEEBE2-94B5-4CA8-AEED-1912D414E515}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Name</t>
   </si>
@@ -37,6 +37,9 @@
     <t>WebsiteAddress</t>
   </si>
   <si>
+    <t>Username</t>
+  </si>
+  <si>
     <t>Address</t>
   </si>
   <si>
@@ -61,74 +64,59 @@
     <t>ContactEmail</t>
   </si>
   <si>
+    <t>PrimaryColor</t>
+  </si>
+  <si>
+    <t>SecondaryColor</t>
+  </si>
+  <si>
     <t>ClientCode</t>
   </si>
   <si>
-    <t>Divine international</t>
-  </si>
-  <si>
-    <t>Divine Internation</t>
-  </si>
-  <si>
-    <t>www.divineschools..ng</t>
-  </si>
-  <si>
-    <t>14, Nile Road</t>
-  </si>
-  <si>
-    <t>Lokoja</t>
-  </si>
-  <si>
-    <t>Koji</t>
+    <t>Straight Gate High School</t>
+  </si>
+  <si>
+    <t>Straight gate High School</t>
+  </si>
+  <si>
+    <t>www.stgh.com</t>
+  </si>
+  <si>
+    <t>SGHS</t>
+  </si>
+  <si>
+    <t>Shomolu Bariga</t>
+  </si>
+  <si>
+    <t>Shomolu</t>
+  </si>
+  <si>
+    <t>Lagos</t>
   </si>
   <si>
     <t>Nigeria</t>
   </si>
   <si>
-    <t>Ola</t>
-  </si>
-  <si>
-    <t>Waju</t>
-  </si>
-  <si>
-    <t>sassasas@mmas.c</t>
-  </si>
-  <si>
-    <t>asasas</t>
-  </si>
-  <si>
-    <t>Fareed law School</t>
-  </si>
-  <si>
-    <t>www.dsseschools.com</t>
-  </si>
-  <si>
-    <t>24, Malam Nile Road</t>
-  </si>
-  <si>
-    <t>VI</t>
-  </si>
-  <si>
-    <t>lagos</t>
-  </si>
-  <si>
-    <t>Fareed</t>
-  </si>
-  <si>
-    <t>Babalola</t>
-  </si>
-  <si>
-    <t>s@dusdu.com</t>
-  </si>
-  <si>
-    <t>A12121212</t>
+    <t>Jekili</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>jones_jekili@stgh.com</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Indigo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +128,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -166,9 +162,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -484,21 +481,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" width="43.140625" customWidth="1"/>
-    <col min="10" max="10" width="36.42578125" customWidth="1"/>
-    <col min="11" max="11" width="49.42578125" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="3" max="4" width="43.140625" customWidth="1"/>
+    <col min="5" max="5" width="45.28515625" customWidth="1"/>
+    <col min="9" max="9" width="23.7109375" customWidth="1"/>
+    <col min="10" max="10" width="22.28515625" customWidth="1"/>
+    <col min="11" max="11" width="36.42578125" customWidth="1"/>
+    <col min="12" max="14" width="49.42578125" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -535,89 +537,64 @@
       <c r="L1" t="s">
         <v>11</v>
       </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2">
-        <v>9098328782</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="J2" t="s">
         <v>24</v>
       </c>
-      <c r="D3" t="s">
+      <c r="K2">
+        <v>9045671234</v>
+      </c>
+      <c r="L2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E3" t="s">
+      <c r="M2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F3" t="s">
+      <c r="N2" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3">
-        <v>98988777666</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{EF7DF655-FAA2-4FD4-8107-A325B6B7931F}"/>
-    <hyperlink ref="K2" r:id="rId2" xr:uid="{1B0A09DF-551E-4A7A-8FF5-74778312F4A4}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{A5CEBC77-D047-4CEA-90E4-FE8DD5A66A0C}"/>
-    <hyperlink ref="K3" r:id="rId4" xr:uid="{DE43C83D-A438-439B-ABAE-F3260DF77DDD}"/>
+    <hyperlink ref="L2" r:id="rId2" xr:uid="{1B0A09DF-551E-4A7A-8FF5-74778312F4A4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>